<commit_message>
Get daily reddit data: Tue Oct 15 08:11:02 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_20.xlsx
+++ b/data/collected_data/2024_10_20.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C512"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3593 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1g42ass</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t xml:space="preserve">French nails for the first time. Hit or miss? </t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/axd30j8iivud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1g41c2o</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Terrifier Inspired Nails for Halloween</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g41c2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1g41t9q</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Subtle Halloween 🦇✨</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g41t9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1g41cpj</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>anyone know the base pink color or one that is like this? thanks</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s3zlpfsi5vud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1g419fl</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vampy bite </t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y25ntfsa4vud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1g4015k</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New spaceship nails! I saw someone post these a few weeks back and had to copy them. To whoever originally had these thank you for the inspo. I get excited everytime I look at them! </t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dcih595cpuud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1g3zta6</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What nail shape for acrylics would be best for being able to do daily life activities? </t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g3zta6/what_nail_shape_for_acrylics_would_be_best_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1g3zrcz</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Zoya Beth </t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dblud4mdmuud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1g3zr3q</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>I redid them (just one hand)🤣</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3zr3q</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1g3zejs</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Reminder: nail art is so much harder and time consuming than it looks</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s3vx9mjhiuud1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1g3z6ii</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>The juice is loose! 🪲💜 These took a while but I’m so pleased with the outcome 😊</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3z6ii</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1g3z154</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stuck! </t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3z154</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1g3yxny</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Should I change my nails color back to black? :3</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1i9si355uud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1g3yuye</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need tips for best way to adhere my own press-on nails. </t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g3yuye/need_tips_for_best_way_to_adhere_my_own_presson/</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1g3yd0t</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>selling press-ons</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g3yd0t/selling_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1g3y8af</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Love my new nails 😍</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xnh45k2m6uud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1g3y8fg</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Gel keeps lifting</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g3y8fg/gel_keeps_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1g3xsnl</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Eye-conic Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3xsnl</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1g3xpon</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Classic Spooky Drips for Halloween </t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q66sk9ys1uud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1g3xn5k</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Pastel Halloween vibes ofc</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3xn5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1g3xckz</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>My Favorite Season is Fall</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sbh8y9ieytud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1g3xhmg</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Witchy nails for October</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vw1pk14qztud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1g3xds6</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink halloween spider webs </t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k5d3rkqpytud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1g3wqvm</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Freshly done 🤍</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bgs3w5wtstud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1g3woif</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>I love these 🥹</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3woif</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1g3vuvx</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Builder Acrylic </t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g3vuvx/builder_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1g3vp2v</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Dior Abricot - Creme vs. Serum</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g3vp2v/dior_abricot_creme_vs_serum/</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1g3vlt4</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>43 year old husband and farther here. How did I do?</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bkxkcp7eitud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1g3v1g5</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Halloween nails</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7lr0lzofdtud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1g3u3v7</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Halloween nails</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2psejzf75tud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1g3tvby</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Press on with gel</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g3tvby/press_on_with_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1g3tly7</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What shape would suit me best? </t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3tly7</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1g3svvr</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Vampy Vibes🧛🏼‍♀️🖤♥️</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/igydx1drusud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1g3sulf</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Nice!</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ojs8f74husud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1g3rosk</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black widow polish for October </t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3rosk</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1g3g1el</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>How to go about my next appt</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g3g1el/how_to_go_about_my_next_appt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1g3jlii</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>My acrylics have been growing out differently for a while and I feel like it’s not supposed to look like this…?</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3jlii</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1g3ozw2</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I've tried so many brands. </t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g3ozw2/ive_tried_so_many_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1g3red4</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>I decided on a basic design, because I work a lot and I can't take care of them so much.</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3red4</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1g3r8cw</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>What do you think of this color?</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ki2qu0eehsud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1g3qgpl</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Is a polish change possible w/ 3D art?</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cvg3v3hsbsud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1g3qbr2</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>My birthday nails🥹🥹</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5xqpk7xrasud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1g3qavi</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>My Halloween set ✨🕸️🌙</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r9tmngtlasud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1g3pwsa</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got some spooky ghosts done for Halloween </t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3pwsa</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1g3pqxa</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>How were my nails?</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fe2z2jbg6sud1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1g3paue</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Getting closer to the Pinterest pictures </t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3paue</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1g3pcf1</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New acdylicd! I gave my nails a few months break.. sooo glad to have my acrylics back! </t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zpaeuv5i3sud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1g3pay5</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>How to Remove Gel X? Without damaging the design.</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g3pay5/how_to_remove_gel_x_without_damaging_the_design/</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1g3ow6b</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Struggling to find flattering neutral nail polish colors?</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3ow6b</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1g3oq6w</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Embracing The Imperfection My Journey to Loving My Hands And Nails</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6isn92b2zrud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1g3ol1t</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>halloween nails !! 👻🕸️</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3ol1t</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1g3ofeq</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Sally nails!</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3ofeq</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1g3o2kh</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BIAB separating from nails after two weeks </t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3o2kh</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1g3nwcj</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Took a stab at ghost nails! 👻 I used glow in the dark acrylic</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3nwcj</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1g3nn0d</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Nail Reformation has the best press ons😍</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ututeh3rrud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1g3n11h</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>First time doing my own nails</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3n11h</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1g3n7k8</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>My new Halloween set 🩸👻🩸</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3n7k8</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1g3ned1</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Cat eye is my new favourite! (Franko approves)</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8xq404cprud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1g3mn4u</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>little basic but im so in love😍</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4v42zkmtjrud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1g3mkki</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>I'm so nail salon dumb, help me</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g3mkki/im_so_nail_salon_dumb_help_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1g3lx0s</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>18 months of nails! Which are your favourites?</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3lx0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1g3lca1</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Advice for Straighter Lines?</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3oa6a1harud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1g3l9ny</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall cat eye nails 🍁 </t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3l9ny</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1g3l7b5</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Will I be able to get gel/BIAB over this nail break?</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3055ubdi9rud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1g3l362</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🕷 nails </t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wjjc1po8rud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1g3kp3y</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Halloween Nails ❤️</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uugqy6nw5rud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1g3jolz</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>What I asked for v what I got no</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3jolz</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1g3kica</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>OPI Black Cherry Chutney 🍒🖤</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eh23wnqi4rud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1g3kf76</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Clean girl halloween nails!</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3kf76</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1g3kdh4</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>nail advice</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o22dtj7j3rud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1g3k9bv</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing this kind of design 🩸 </t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fablsg3r2rud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1g3k8ue</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>🍁✨</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3k8ue</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1g3k0my</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Nail Tips</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3k0my</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1g3jxrv</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I can’t decide if I like these or not.. Opinions please! </t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3jxrv</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1g3jqsk</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got these done for a wedding! </t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ugyr7vbyyqud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1g3jii8</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>This weeks messy mani</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3jii8</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1g3exlb</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>My DIY pink aura nails for Breast Cancer Awareness</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5x2yis8fxpud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1g3ba60</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Applied 3 days ago and nearly all are off. I'm using BIAB. Please help. </t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3ba60</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1g3aq1l</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Green/blue gel aurora nails</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3aq1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1g3jkms</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky nails🎃🧡 </t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3jkms</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1g3jj85</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Funky mushie 🍄nails💜</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wr02ishexqud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1g3jawt</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>First time doing my own nails</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfnt9onpvqud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1g3j1ol</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should i go almond for this color of polish or stick to my always coffin? </t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3j1ol</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1g3i96o</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Halloween but make it 🩷🎀🌸</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3i96o</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1g3hkvn</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>SPOOKY SZN 🩶</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3hkvn</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1g3hk7r</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Antique-y Pumpkins</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3hk7r</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1g3hiys</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>I think I didn't know how to do the gradient very well 🥹</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l6xj6yjiiqud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1g3haxa</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Non conventional bridal nails</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3haxa</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1g3glsy</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Spooky season nails! Inspo from @nail.brat</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3glsy</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1g3g8wi</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Scary Cute 👻</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2zbzuqrk8qud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1g3g7xb</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>I love it</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2kqzvvyc8qud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1g3g679</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>my nail tech drew every single part of these by hand, HOW are people this talented??? 😭😭😭</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3g679</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1g3fqoa</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>In love with my new design 😍</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdh574oe4qud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1g3fm75</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>I love painting my French manicures myself 😍</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jl4hnm8c3qud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1g3f591</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>what do we think? 👻</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3f591</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1g3ecii</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Spooky nails are the best nails 🦇</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvg3yic6spud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1g3eb2o</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>New autumn set I made</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3eb2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1g3cxve</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Strawberry Matcha🍓🍵</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3cxve</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1g3cr6h</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why do some of my nails curve while others grows straight? </t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/31dyz4l3apud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1g3cpkm</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>vampy nails</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3cpkm</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1g42n66</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Can you use Essie gel couture if you’re allergic to real gel?</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g42n66/can_you_use_essie_gel_couture_if_youre_allergic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1g40u0r</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Bewitched and Venom</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g40u0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1g40d7y</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The 'Lazy Wench' Metallic Mani 🤷‍♀️ </t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/10-10-2024-GxWoniY</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1g40az4</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>How to turn into a real zombie for Halloween- wear dark polish. 🧟‍♀️ Wear a light colored polish on pulse ox monitoring finger. ((Swipe for difference between light and dark))</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g40az4</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1g3zpt1</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>New favorite</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3zpt1</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1g3zkmm</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>2nd gel set</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x9ympzlbkuud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1g3zj5g</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>2nd attempt at magnetic gel, this time attempted “glass” look</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1163jsbqjuud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1g3z5u9</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Grass Knot</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3z5u9</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1g3ymyb</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>new subreddit for dazzle dry!</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/dazzledry/s/LQmwrmI17P</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1g3yh80</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Polish dupe for Color Street Tokyo Lights?</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3yh80</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1g3yg4d</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Drugstore Layering</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3yg4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1g3y70e</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Red/black thermal polish Halloween ideas</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g3y70e/redblack_thermal_polish_halloween_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1g3xfwv</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Looking for a good nude gel polish preferably a more opaque one</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g3xfwv/looking_for_a_good_nude_gel_polish_preferably_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1g3x62s</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Spooky-cute mani 🦇✧🔮⋆🎃</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yiyz55uxvtud1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1g3wlf5</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>burdock &amp; buckthorn ✨</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3wlf5</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1g3w4j6</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Y'all I swear the camera does not do this polish JUSTICE</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3w4j6</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1g3vxui</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>I just realized I matched my polish to my cat</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3vxui</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1g3v1wm</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t xml:space="preserve">wildest color i’ve done! </t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dd13ukijdtud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1g3uyco</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Polish decals</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g3uyco/polish_decals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1g3uvfy</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Chamaeleon Nails just earned themselves a screeching, simping fangirl 💣</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3uvfy</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1g3upte</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>What could have caused Onycholosis? (product-wise)</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g3upte/what_could_have_caused_onycholosis_productwise/</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1g3u3ce</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>mooncat moonflower</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vla6dim35tud1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1g3udvy</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome powder reaction/allergy? </t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3udvy</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1g3twxl</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail art brush w/cheap shipping to Canada </t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g3twxl/nail_art_brush_wcheap_shipping_to_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1g3ts7a</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>beetles on press ons?</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g3ts7a/beetles_on_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1g3tn5q</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>my very simple vampire manicure on my shorties 🦇</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3tn5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1g3tbwg</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Developed gel allergy but not from DIY nails. Any idea what could’ve happened? </t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g3tbwg/developed_gel_allergy_but_not_from_diy_nails_any/</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1g3tbgc</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Indie polishes</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g3tbgc/indie_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1g3t4uy</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>An attempt at fire Opal nails</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3t4uy</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1g3sl9l</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Hidden Potential has no right to be this beautiful 🌧</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ei7835j9ssud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1g3s6t1</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>KBShimmer "I Can't Decider"</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3zor7yhzosud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1g3rwyg</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Help me with a good shape!</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3rwyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1g3rvn9</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Pls help me choose a shape</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3rvn9</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1g3rtit</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>🍃🫶Heart Stopper🫶🍃</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3rtit</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1g3rjjt</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Halloween nails to match my Halloween cardigan 🎃</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3rjjt</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1g3rign</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Tried something new and I love it</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3rign</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1g3r8q6</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>First time using a thermal polish 😍</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3r8q6</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1g3qzz2</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hurricane nails! </t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3qzz2</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1g3ql0y</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>🌺🍁</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3ql0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1g3pffv</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Does regular polish need to be kept out of light?</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g3pffv/does_regular_polish_need_to_be_kept_out_of_light/</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1g3ol5s</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Similarities: Cirque Colors vs Mooncat October 2024</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3ol5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1g3odex</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>(potential) gel polish allergy, and getting braces - are these ingredients going to be problematic like adhesives used for crowns?</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgwcoejgwrud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1g3nizx</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Unintentionally matched my flannel to my nails today</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aq7qmcm9qrud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1g3n8xj</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>OPIxWicked Ozitively Elphaba</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3n8xj</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1g3n846</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Apple Of My Eye 🍏🌟</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vzhtcqw0orud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1g3n7sz</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Bad manicure?</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3n7sz</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1g3mxe4</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>birthday nails: OPI feelin' libra-ted 🥳🎉🎈</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3mxe4</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1g3msl2</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Dainty floral</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ukcsh4ozkrud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1g3mqxy</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Earth to Gaia is so underrated!</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3mqxy</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1g3mojh</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Gave myself some fall nails from Holo Taco!</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/05unqwlqirud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1g3miqr</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Cirque Fool's Paradise</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3miqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1g3mcmc</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Clionadh :: Prototype</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3mcmc</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1g3m871</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for recommendations </t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g3m871/looking_for_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1g3m02n</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>In love with this dark red</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3m02n</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1g3lzjw</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Trick or treat</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ujwnpp4frud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1g3lmq3</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Velvet without 30lb magnet? </t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g3lmq3/velvet_without_30lb_magnet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1g3lj19</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mean Ghouls - Polished for Days </t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gedh6d9sbrud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1g3l54o</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cracked Polish Leather Bound </t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3l54o</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1g3l341</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Spooky Season shorties!</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74j52kfl8rud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1g3klyr</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BKL Stronger Together </t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3klyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1g3kek7</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>ILNP's Pool Party is magical</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9njr1zop3rud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1g3k7bt</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EDM Haunted Vibes </t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ph8ehwb2rud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1g3k42l</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what do these remind you of? hand painted by me! (__kmnails) </t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4q258iso1rud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1g3k3v3</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Recreating a discontinued polish</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/imoazm5n1rud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1g3k1zc</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t xml:space="preserve">halloween but make it girly! hand painted by me (__kmnails) </t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f4mnpuc91rud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1g3jxpe</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Mooncat new shade names</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hdmrmsvd0rud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1g3juys</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Supervillain isn’t hitting the spot. </t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3juys</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1g3jl06</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Are my nails suited for almond?</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hkzgnierxqud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1g3io7x</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>This weeks messy mani</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3io7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1g3ijs4</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>ILNP’s Venom is such a great spooky shade. 😍🐍🧪</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3ijs4</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1g3if0d</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Bubbles 🫧 </t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3if0d</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1g3ieul</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>how dangerous are allergies to gel nail polish?</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g3ieul/how_dangerous_are_allergies_to_gel_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1g3ia0d</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>CD Rom-antic 📀</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcxdfo85oqud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1g3hgwe</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>ILNP Birefringence &lt;3</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3hgwe</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1g3gsoy</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>ISO navy creme nail color</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g3gsoy/iso_navy_creme_nail_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1g3fb5t</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What causes peeling in nails? </t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g3fb5t/what_causes_peeling_in_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1g3f01c</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Throwback polish - and why I stopped using OPI</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wlsla761ypud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1g3es3m</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Tbh, disappointed. Am I crazy?</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xl92f4n2wpud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1g3c9l6</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g3c9l6/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1g3buqj</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>BEST/most blingy Glitter or holo glitter polish?:)</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g3buqj/bestmost_blingy_glitter_or_holo_glitter_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1g3b1ag</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Thermals are too fun</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikdv2dzhmoud1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1g42oyd</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Flowers and feathers nail art tutorial</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1g42oyd/flowers_and_feathers_nail_art_tutorial/</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1g426ri</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1hour to done my job </t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ckikh3uugvud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1g40v7u</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried to make this set </t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1crb0e0azuud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1g3zjom</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to get “glass” look with magetic gels!? </t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p2ydgfwvjuud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1g3zik0</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY: 2nd attempt tried two magnetic styles </t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xwtycw1kjuud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1g3ywe6</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love my new nails! </t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m9tqjyz6duud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1g3y5gn</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>🕸️🕸️🕸️</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/piwavn0v5uud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1g3x4w8</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>just started doing gel press ons, i’m so proud of these so far!🤍</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3x4w8</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1g3v8rg</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Horror Movie Nails - credit Kim</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3v8rg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1g3u5f9</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky season </t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/som7hhdk5tud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1g3tsg7</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>✨ Harry Potter nail set for this Halloween 🎃</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3tsg7</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1g3senl</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Gel manicure and stars</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9en3g20uqsud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1g3s76j</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Halloween Inspo</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3fv7f5c5psud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1g3rrsf</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Brand new Halloween nails!</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k3gxsvctlsud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1g3r92v</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>I’m redoing the set. 😶‍🌫️</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q1vnjfnohsud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1g3qeri</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Very cute, I loved them!</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hbb24xz7bsud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1g3qdh9</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>My birthday nails 🥹🥰</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sthcwsn4bsud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1g3q5kc</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>The time of villains is Halloween</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lmwmnh4i9sud1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1g3q0cy</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving these Halloween designs!! 🔪🩸 </t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcf9xv6e8sud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1g3p18l</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Y2K nails 💅 First time doing tiger stripes it was so hard! These are press on nails :) </t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zm0dhih81sud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1g3oc63</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>My Halloween nails 👻</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cg19ohs7wrud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1g3mxiw</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bird mani with regular nail polish </t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3mxiw</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1g3mw08</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>For art across multiple nails, do you line up tips or cuticles?</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1g3mw08/for_art_across_multiple_nails_do_you_line_up_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1g3lezc</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Advice for Straighter Lines?</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/99n3uve0brud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1g3jq7m</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>My recent competition entry for the theme "Goth" (and I came 3rd, woo!!)</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9n5cnluyqud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1g3h7ja</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>My favorite nails in a long time. The base is temperature changing from clear to Black, then green purple magnetic polish on top. The blotchy finish is packing materials and a jelly stamp.</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3h7ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1g3h22m</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Minecraft nails!!! </t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3h22m</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1g3gyh0</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Scary Cute 🎃</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bfwlf1g6equd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1g3ebmm</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New cat eye nails. (Cat approved) </t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ldva87txrpud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1g3did4</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Just wanted to update about my wedding nails if allowed. They did grow on me after a couple hours and of course I didn’t really think about them the day of 😅 thanks for the kind words, y’all! 💕</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g3did4</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Oct 16 08:10:49 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_20.xlsx
+++ b/data/collected_data/2024_10_20.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C512"/>
+  <dimension ref="A1:C679"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9137,6 +9137,2845 @@
         </is>
       </c>
     </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1g4u4n7</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my girl's nails for twitchcon last month </t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ylijxg8r2vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1g4tura</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Nail stickers are a thin coating for pedicures</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vusw4pjdn2vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1g4tlia</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Razor nicked my gel manicure</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2vod9b2sj2vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1g4rnbe</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails </t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6rtsfm5v1vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1g4s8cl</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Had to share this devil kewpie I did today! </t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c919xga022vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1g4s8u2</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Electric file tips for beginners </t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g4s8u2/electric_file_tips_for_beginners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1g4sd05</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>How do you make hard gel extensions last</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g4sd05/how_do_you_make_hard_gel_extensions_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1g4su6k</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Short nail beds</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y2k3uhxp92vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1g4scem</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>felt cute, asked them to match my sweater x</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84a0u1ed32vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1g4rhvv</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to get rid of turmeric stains? </t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g4rhvv/how_to_get_rid_of_turmeric_stains/</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1g4rfl3</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>First attempt—how did I do?</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4rfl3</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1g4rcb9</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Baby’s first broken nail </t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wudbglmir1vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1g4raio</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can’t tell if identity crisis or objectively bad nails </t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4raio</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1g4r8wd</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t xml:space="preserve">After some filing </t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4r8wd</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1g4r05k</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Not exactly birthday nails…</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5eps6dctn1vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1g4oic2</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question about regular polish over acrylics </t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g4oic2/question_about_regular_polish_over_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1g4lm23</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Best nude color on me?</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4lm23</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1g4qxgy</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Brand new ✨</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4qxgy</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1g4qvb8</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails </t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ypedu03dm1vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1g4qprt</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>I tried the scary nails too 🧟‍♀️</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4qprt</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1g4qli4</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween Nails 👻 </t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8rgd9e4ij1vd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1g4pl23</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Killer nails, killer seal</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4pl23</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1g4p4w2</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Custom press-ons by yours truly 😘</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ta7qa5p051vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1g4omks</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for a gel polish with similar color to this! </t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8g8f4i9a01vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1g4nn5g</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Did these for my MIL tonight. She loved them!</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzprcjo1r0vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1g4mltz</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just had these done and love them! 👻 </t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jm5s6vrh0vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1g4mlcl</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4mlcl</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1g4j5u7</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>October nails 2024</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g4j5u7/october_nails_2024/</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1g4lops</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Looking for OPI color list by number</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g4lops/looking_for_opi_color_list_by_number/</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1g4mh6b</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Did the gel on myself. I’m not a pro, please don’t judge too hard</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rs6cqj4ng0vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1g4megi</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>These took me ages. They not perfect but I love them</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3vlbof6zf0vd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1g4m82r</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Fall nails. Perfect for carving pumpkins. 🎃 😆</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9piae3uee0vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1g4m7dv</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New home studio for my celebs clients. </t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxjlfh39e0vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1g4m5ug</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Moonlight nails for fall</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ossl2i2vd0vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1g4lpa3</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Fall so far ❤️🤎</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4lpa3</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1g4li5z</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Another OPI Gel Mani  my</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4li5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1g4lg75</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need help with nail shape- never had a manicure before </t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4lg75</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1g4l67v</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>October nails 😍</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/enxnyqs850vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1g4l0pb</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Ok I have another builder gel question</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g4l0pb/ok_i_have_another_builder_gel_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1g4kr2y</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Grey</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1zooupop10vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1g4k6c3</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Cake Day Halloween Nails 🎂👻</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bk485ftxwzud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1g4jyqn</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Not bad for being SHEIN press-on’s 🤷🏻‍♀️💅🏼 lol</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s04nfka7vzud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1g4jlfx</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I don’t usually get nail art but how did my nail tech do? </t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4jlfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1g4jl31</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Marbles 🥰</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4jl31</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1g4jdem</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Spooky season. Do you like it?</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0erkylxdqzud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1g4jb8i</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Yay or nay? Don’t ever really do this color </t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69naek3xpzud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1g4j9cm</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>First practice set I’ve done on my own hands !!</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l79ummqgpzud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1g4j6vv</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The most adorable set everrrr.  </t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rnjten6yozud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1g4it8i</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ghostie nails 👻 </t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4it8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1g4ievh</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Spoopy</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4ievh</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1g4i979</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Re: Am I Nail blind? </t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4i979</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1g4ho9z</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>How to improve it??</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jybh3cgcdzud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1g4hmxi</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>shittily painted but i love the color for october</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0gk5qew2dzud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1g4hjfh</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Fall Nails 💅 (Polygel Edition) Last slide was the mood for the appointment🍷😂</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4hjfh</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1g4hf25</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Red is so hard to clean omfg 😮‍💨</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pwpo9vbfbzud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1g4hea4</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A love an iridescent nail moment! </t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hst20li9bzud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1g4h0ud</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Red acrylics, what color pedicure??</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g4h0ud/red_acrylics_what_color_pedicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1g4gz96</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>these are so cute 😍</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8567hrq28zud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1g4gwkr</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>can i get a hell yeah for fall nails? 🗣️</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/akmtqwoi7zud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1g4gc1s</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Can I use acrylic to fill in my grown out gel press-ons?</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g4gc1s/can_i_use_acrylic_to_fill_in_my_grown_out_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1g4gatz</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why does this happen when I paint my nails? </t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b6yg0hny2zud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1g4g5c7</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Be honest are they cute or no 🥺🤣</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ssasths1zud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1g4fv7o</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The nightmare before Christmas </t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u8qwgzdnzyud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1g4fiyr</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sistaco review buyer beware </t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4fiyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1g4f790</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Added a 3d flower and snake to my fairy nails.. But idk if i like it. </t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4mb5sgouyud1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1g4f6m5</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Press on nail: don't use the sticky stickers</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kyppnq5juyud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1g4f1bt</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Love this baby blue, aqua, &amp; copper glitter!</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4f1bt</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1g4et8b</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Pour one out for my natural nails. They’ve never been this long and this healthy, and I’m about to chop them off.</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4et8b</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1g4e166</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Not sure how I feel about this color.</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4e166</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1g4dygo</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall nails 💅  what do u think ? </t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ij8lakgclyud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1g4co9c</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Is this normal experience?</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g4co9c/is_this_normal_experience/</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1g4d5gq</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Broke my natural nail due to too-thin builder gel, what to do?</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mv6k1m5afyud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1g4coid</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Please help me pick gel nails brands !</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g4coid/please_help_me_pick_gel_nails_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1g4dial</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cute set I did for my bestie </t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g36b2i0yhyud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1g4dg8h</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t xml:space="preserve">exid! &lt;3 </t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60nu4w8ihyud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1g4d74k</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Update on my previous post of short wonky french nails</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4d74k</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1g4d0k0</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Soft green and gold set</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4d0k0</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1g4cxkq</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Having a really good nail day</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hs0mjbndyud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1g4crp0</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Gel x - is this normal</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4crp0</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1g4coqt</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Just got a new mani, i have my feets done on the same colour and detail. 💖</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5uc1h6tbyud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1g4cc7u</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Manicure for autumn mood  </t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2uqtli479yud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1g4c2pu</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall nails </t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i2gtughb7yud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1g4bzt7</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Japanese gel salon in NYC or North NJ?</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g4bzt7/japanese_gel_salon_in_nyc_or_north_nj/</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1g4bt8i</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Eyeing my nails</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4bt8i</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1g4bsaw</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>My witchy fall nails</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4bsaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1g4bfio</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>2nd gel attempt</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7t3xyof2yud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1g4audm</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Uneven nails , blooming gel advice please 🥲</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4audm</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1g4an94</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Bloody Nails</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4an94</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1g440cz</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Throbbing pain from acrylic nails? </t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g440cz/throbbing_pain_from_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1g4a1j0</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween Nails </t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/atc4pin0sxud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1g4a0k7</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Everyone's favorite classic</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gvoy14dqrxud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1g49gc0</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails </t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g49gc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1g48kjd</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>I wanna cry. Asked for long nails and got this mess. 45€ in the bin</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g48kjd</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1g481q4</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Out of my comfort zone</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yeng5928cxud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1g470hp</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Am I nail blind? </t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g470hp</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1g46xrf</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Nailcare tips</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g46xrf</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1g43cxw</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What should I start with as someone with next to no experience with nail polish etc? </t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g43cxw/what_should_i_start_with_as_someone_with_next_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1g4uaf1</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Love this colour in the bottle but I'm not sure it suits my skin tone. What do we think?</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1s0o6xsht2vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1g4tzk1</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Nailed It! “I’ve Seen Betta Days” (02/24 PPU)</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4tzk1</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1g4renk</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Any light shades of pink that don’t make me look washed out or yellow?</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g4renk/any_light_shades_of_pink_that_dont_make_me_look/</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1g4rcsf</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DND gel &amp; chrome powder </t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g4rcsf/dnd_gel_chrome_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1g4p8l1</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Help me decide between 2 similar shades :)</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tarp6zq161vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1g4p4uw</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Never done square nails before but I broke a nail and decided to run with it</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4p4uw</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1g4otx1</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Dupe requests for this shade?</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g4otx1/dupe_requests_for_this_shade/</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1g4oqkw</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Pumpkins and grave soil 🎃🪦</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gj6n7f2911vd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1g4ok3t</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Solar prugly? ☀️🤢</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4ok3t</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1g4oe57</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Why are the bases of some of my nails clear (the clear parts are also less strong and bend in)</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/meeltc35x0vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1g4odob</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to avoid breaking nails? </t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4odob</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1g4o9us</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall Abstract </t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4tgrb2yw0vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1g4o6ek</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>So mad at myself for taking a full YEAR to try this beauty 🤦‍♀️</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4o6ek</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1g4nsf9</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Mooncat Nocturne - First Time Magnetizing!</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pduqggrfs0vd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1g4m15e</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Need more recommendations for lip gloss finish polishes - obsessed with ILNP Pixie party and flower child</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g4m15e/need_more_recommendations_for_lip_gloss_finish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1g4ls4o</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>My first Rogue Lacquer order</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4ls4o</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1g4l69i</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>It's giving graveyard, right?</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/72k7ir5950vd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1g4ke6u</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Got distracted and did a photo shoot when I should be studying 😂</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4ke6u</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1g4ju5u</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>You Are The Rock That Refuses</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fwpaaoe6uzud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1g4jqm3</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Psilocybin vs Bill</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fvnkemebtzud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1g4jme2</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Dupe request for ”Lucky Clover” by Drunk Fairy Polish</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5p35nzeszud1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1g4jar6</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>ILNP Lily</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4jar6</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1g4id00</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>I chose this color to match her eyes 😻</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4id00</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1g4hzd0</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Favorite ILNP multi chrome polishes?</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g4hzd0/favorite_ilnp_multi_chrome_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1g4hquz</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Swatch request!</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g4hquz/swatch_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1g4hkcv</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Looking for a non gel alternative to the builder gel by in.hype cool nude 6.</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4hkcv</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1g4hk1r</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Duochrome &amp; holo is the way to my heart 💜💙 (Gifted PR) - details in comment</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4hk1r</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1g4gnts</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Day 10 manicure show off!! </t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rl5i06lo5zud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1g4g15z</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sheer pink jelly polish recommendation </t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g4g15z/sheer_pink_jelly_polish_recommendation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1g4fwwn</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>matched my nails to my boyfriends car</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j39j73110zud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1g4ff4t</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I need help - brittle nails that break down the middle </t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4ff4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1g4faaa</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>👻Ghost French Tips👻</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4faaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1g4ezq8</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Custom press-ons made by yours truly 😘</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/br4sx6b4tyud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1g4ez0a</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP Happy Hour vs Mooncat Fake Halo swatch request </t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g4ez0a/ilnp_happy_hour_vs_mooncat_fake_halo_swatch/</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1g4evp4</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Written invitation </t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4evp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1g4ef47</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Chilly greys and spooky days</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4ef47</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1g4dvoj</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hobbiest here, designs won’t stay put </t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6r55w3rkyud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1g4dtzu</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I have no yellow polishes. Suggest me one that will make me love yellow </t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g4dtzu/i_have_no_yellow_polishes_suggest_me_one_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1g4dbsw</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>i need less expensive hobbies</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3sjwcjkgyud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1g4d2wn</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Starting to love my shorties!</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hn60zwiqeyud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1g4cx29</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Having a really good nail day </t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gcjz0gpjdyud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1g4cwmn</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>I’m that bat bitch</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qibkgtagdyud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1g4csy2</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Experimenting with adding isopropyl alcohol with thinner to my topcoat</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g4csy2/experimenting_with_adding_isopropyl_alcohol_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1g4cdv7</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tis’ fall 🍂 </t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4cdv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1g4cajr</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Death Angel</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4cajr</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1g4bs5p</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Sparkly blood</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n2qkjlz05yud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1g4bc22</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Uneven nails , blooming gel advice please 🥲</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4audm</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1g4angr</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Pumpkin Vibes🍁</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4angr</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1g4a0l8</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Help me find this color!</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ra4doxotrxud1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1g49u42</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Has anyone tried making their own topper with topcoat/clear polish? Would this work?</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g49u42</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1g48jpj</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What am I missing? </t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/63jjjpabgxud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1g46i5n</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Had a little 🔪 accident today </t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hofkje1sywud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1g45o47</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>DVN Pearls on Mars</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g45o47</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1g4tk71</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Anyone is interested in this nails design?</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hibnfg93j2vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1g4s0le</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Had to share this devil kewpie I did today! </t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0xph4qez1vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1g4qwbm</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Halloween nails</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/92d98oaom1vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1g4p9gj</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Halloween set help!</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4p9gj</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1g4p5d3</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>GLOWORM NAILS!!!</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n25qa51451vd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1g4jbw8</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>I did them with my friend IG: @yonahilisramirez</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w83ep492qzud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1g4izlf</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2 years ago vs today </t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4izlf</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1g4in00</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Love me some spiders</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4in00</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1g4ifbe</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Favorite everything?</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1g4ifbe/favorite_everything/</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1g4i6wv</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eye green love it </t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ylyg9a88hzud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1g4dtjp</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Designs smudge every time </t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/38rz8fiakyud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1g4d2em</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Soft green and golden set</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4d2em</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1g4br98</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>I saw these on insta and had to do them for myself (inspo at the end)</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4br98</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1g4aufh</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails in acrilic with strass </t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/52vh6892yxud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1g49l05</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>6 months of improving my brush technique 🦋</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g49l05</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1g48rup</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>✨Who's that Pokemon?</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lnw7vyd3ixud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1g43x1h</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Flowers and Feathers nail art tutorial</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zj5ezya06wud1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Oct 17 08:11:13 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_20.xlsx
+++ b/data/collected_data/2024_10_20.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C679"/>
+  <dimension ref="A1:C841"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11976,6 +11976,2760 @@
         </is>
       </c>
     </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1g5flj4</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Kiss nail glue won't release my natural nails. My natural nail is half broken from the nail bed and I can feel pain when I try to pry the false nail off. Tried everything</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g5flj4/kiss_nail_glue_wont_release_my_natural_nails_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1g5klxa</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Tips on doing Gel-X at home</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g5klxa/tips_on_doing_gelx_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1g5kog3</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Feelin’ the Bluesss</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5kog3</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1g5jrri</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Nail Color Dupe</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g5jrri/nail_color_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1g5k7h0</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Halloween nailsss 👻</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5k7h0</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1g5k8wy</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First gel set I have ever gotten. Done by me. </t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vsfq52j5c9vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1g5k5y1</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails 👻 </t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5k5y1</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1g5j7ax</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Question about enhancement types?</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g5j7ax/question_about_enhancement_types/</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1g5irvx</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Halloween nails!</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8mituw8v8vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1g5iqkb</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I use this under gel polish to protect the nail? </t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11c8hf7vu8vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1g5imqc</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Trying to buy a gift for my wife</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g5imqc/trying_to_buy_a_gift_for_my_wife/</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1g5ihx4</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Gel-x Nails in Chicago</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g5ihx4/gelx_nails_in_chicago/</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1g5hgya</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall Nails! Inspired by @ataman_olga on Instagram </t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5hgya</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1g5hzg8</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Just did these cuties on a friend 💕</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5hzg8</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1g5hxxb</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Finally getting decent at builder gel</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vll8txjam8vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1g5hn88</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Seeing everyone post on this sub has motivated me to post a set I was really proud of :)</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k672x1b9j8vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1g5h6me</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>What do you call these sticking out on the sides of my nail and how to avoid it</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/54jghlfqe8vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1g5h1rs</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t xml:space="preserve">how’d my nail lady do?! </t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5h1rs</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1g5g2dl</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Halloween nails after a long hiatus :)</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5g2dl</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1g5g0p3</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🖤👻🕷️</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5g0p3</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1g5fvs4</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Almond + chrome appreciation</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5fvs4</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1g5fro5</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>took me 6 hours to do my nails but i’m happy with them ❤️</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5fro5</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1g5fiwe</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>How would you make these nails more interesting?</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5fiwe</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1g5f2yl</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Halloween nails </t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jjpaazmqu7vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1g5epa7</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t xml:space="preserve">obsessed with my nail girl </t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5epa7</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1g5edis</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Dungeons and Baddies 💅🏾</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5edis</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1g5dji7</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Still not sure if I love them or not </t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sd0ztf0ng7vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1g5d84e</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Girly Pink French</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g5d84e/girly_pink_french/</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1g5cpt8</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Beetle juice 💚💜🤍</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zlwl5qga97vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1g5c2if</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>New Halloween Set 👻</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5c2if</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1g5c01o</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>I love when my tech says “we’re doing a mystery mani” 🤡</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cxaq3j8737vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1g5blds</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Appreciation post for this sub💜</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g5blds/appreciation_post_for_this_sub/</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1g5bbri</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I did these on myself and I'm kind of obsessed </t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lrlnrrmx6vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1g5a9zd</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>My new bat French tips</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5a9zd</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1g5a316</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Halloween nails</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1xeoiqqn6vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1g59rww</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>It’s frickin bats! I love halloween!🦇</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7j7sm5dl6vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1g59kx9</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>🎃 Painted Polish 💜Boo, Witch!, 🧡 I'm A Haunt Mess, and 💚 Rise &amp; Slime. The perfect Halloween Lite skittle!</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g59kx9</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1g590sx</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>are these nails cool or too weird and flashy for halloween?</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g590sx</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1g58fad</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>How cute are these nails my cousin's wife did for me</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/te2m1vtab6vd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1g57yzj</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Nail lifted from nail bed</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hryf7sks76vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1g574dc</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to stop acrylic nails damaging my natural nails. </t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g574dc/how_to_stop_acrylic_nails_damaging_my_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1g589r4</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nails I did after a long break </t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g589r4</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1g5883l</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Red devil nails </t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rcffwsvq96vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1g57kl0</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Happy (belated) National Mushroom day October 15th across the pond! 🍄</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0m3w39sk46vd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1g57hty</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why didn’t my tech put the nail back to my cuticle? </t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g57hty</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1g56x6o</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Love these 💕</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g56x6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1g56ouk</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Spooky Glam 💓🕸️👻</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8cpyrzyxx5vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1g56e9x</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>SHEIN press-on nails are… interesting 🤣</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g56e9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1g5645e</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Ghastly, Haunter &amp; Gengar Halloween Set</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pxmfahikt5vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1g55mr9</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Why does my nail keep breaking so oddly?</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g55mr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1g5580n</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Where do I even start</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/plh9rg2ym5vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1g55q7t</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails 🖤 </t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g55q7t</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1g55dfq</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Is this shape unflattering for my chubby hands?</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g55dfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1g557jw</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>My wine red nails</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xsxkzbkum5vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1g4vj0t</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Selling press on nails at markets. Any experience? Thoughts? Tips?</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4vj0t</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1g51eu0</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Jelly Glass Nails</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g51eu0/jelly_glass_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1g54pjo</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>DND top coat &amp; chrome powder</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g54pjo/dnd_top_coat_chrome_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1g54kwd</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you like the color black? </t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eawdbvf4i5vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1g54kll</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Purple coquette </t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g54kll</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1g549lp</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It is the first time I have done this type of design. and I fell in love </t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g549lp</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1g548i0</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Took the acrylics off and went for a coffee toffee theme with my natural nails </t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g548i0</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1g548g4</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Me: I'm not obsessed with Hello Kitty. Also me:</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g548g4</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1g53zl7</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>First time getting into nails</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q4vsclpnd5vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1g53sdh</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Olive and June press on nails</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g53sdh</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1g52r1u</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Anyone know a dupe or similar color?</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g52r1u/anyone_know_a_dupe_or_similar_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1g52nd6</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>New to shaping: At what length do you take the plunge to a more defined almond shape? Is there just an "awkward teen" phase or should I have kept them square until they're long enough to pull off almond? Started rounding things out and realized I don't think I have enough to work with.</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rc6k23z35vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1g52k8q</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>My prom dress is green and my after-prom club fit is black and red. What nails and makeup??</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g52k8q/my_prom_dress_is_green_and_my_afterprom_club_fit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1g52h35</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>What nail shape should I be getting?</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eqa919xm25vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1g52gsr</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Got these to match my Halloween costume</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wmd2xu4l25vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1g51fob</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Always Black, so need accent ideas! </t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i49p61rqu4vd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1g51lcs</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>My Halloween set 🎃 (been a while since I did so much nail art, but they turned out cute)</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fn4de5sxv4vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1g51jkw</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone else do this? </t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ntbgjprjv4vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1g5184z</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Purple Chrome Press Ons</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5184z</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1g50pq3</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>opinions on the empty space french tip trend?</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g50pq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1g4wrl5</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Saw these on Pinterest and wanted to try for myself </t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4wrl5</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1g4y7ne</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>How do I remove this glitter line?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4y7ne</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1g4xkzu</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Hows my Halloween thened nailss?? (Those r my real nails )</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4xkzu</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1g5084a</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>KBShimmer - Gummy A Break (reflective)</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5084a</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1g506p9</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Was going for dark and vampy </t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g506p9</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1g504iw</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>♥️🧛🏼‍♀️🥀✨</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5e61uyfk4vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1g4zpk3</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advise on how to get press on nails to blend into my natural nail when they grow out? </t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hq700ik1h4vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1g4yjaj</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>halloween nails!</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3vr0bj374vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1g4y9aw</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>How would you wear this?</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ze5udvi44vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1g4x64a</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Spooky szn</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3adnj56rt3vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1g4vzmx</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Any advice on nail shaping working with gel polish</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sjpqv607g3vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1g4vtia</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I made my first ever press ons :) </t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4vtia</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1g4vfl1</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Finally been so brave and tried something more special. Im so happy with the results</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/av8c80q293vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1g5keb6</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>One single polish</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g5keb6/one_single_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1g5jxon</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Bat nails...bat nails...na na na na na...</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5jxon</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1g5i9ed</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Polish Expiration Dates</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g5i9ed/polish_expiration_dates/</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1g5grx7</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>ILNP - Pool Party 💕🏊‍♀️ and Hidden Treasure 🔮🪙</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5grx7</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1g5gpb7</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>blood-red nails🩸+ magnetic polish 🖤</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5gpb7</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1g5g8l8</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Not usually into white polish</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5g8l8</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1g5esqe</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Love the Flakies!</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5esqe</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1g5ehjo</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Does anyone know how to get either of these magnetic shapes?</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upzj6oj9p7vd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1g5efzu</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Send me all your thoughts and prayers</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g5efzu/send_me_all_your_thoughts_and_prayers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1g5e217</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Cirque Peach Jelly 🪼</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5e217</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1g5d4cc</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Holo Taco Birthstone Collection</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g5d4cc/holo_taco_birthstone_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1g5d2gr</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>someone here also uses things like iridescent mint in a week, classy mauve next week?</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eiy37lpec7vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1g5b1ux</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prep Your Nails for the Holidays with Modelones Pleascent Nail Care Routine! </t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g5b1ux/prep_your_nails_for_the_holidays_with_modelones/</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1g5af4u</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Favorite smaller brands?</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g5af4u/favorite_smaller_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1g5a92t</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Any tips for restoring nails after years of acrylics?</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nq2she12p6vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1g59y8w</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Zoya Bowie is gorgeoussssss</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ntici8pqm6vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1g59js4</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>🎃 Painted Polish 💜Boo, Witch!, 🧡 I'm A Haunt Mess, and 💚 Rise &amp; Slime. The perfect Halloween Lite skittle!</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g59js4</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1g59fvx</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Clionadh Cosmetics - Hilt</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g59fvx</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1g59c49</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>My fav pink/blue shimmer ♡</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g59c49</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1g58k7q</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP - moonlit </t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2xdc0c6cc6vd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1g58i3z</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Didn't expect to like this color and now I love it</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/enahlhvwb6vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1g58hp4</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>A fiesta blue sneaking in between the Fall colored manis</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g58hp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1g58ezd</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>By Dany Vianna- Sunflowers</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yo0teeh8b6vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1g58aez</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>How do you guys determine what nail length or polish won't work against you in professional jobs?</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g58aez/how_do_you_guys_determine_what_nail_length_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1g581x0</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Mistress- Phoenix ♥️💙</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/eig3c11b76vd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1g57n8i</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Black Friday sales</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g57n8i/black_friday_sales/</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1g57hpy</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Happy (belated) National Mushroom day across the pond October 15th! 🍄</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ch42ojrt36vd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1g57724</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Gel allergy or paronychia?</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49ao6abq16vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1g576oa</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>My shimmery shiny mani is my own private dopamine machine</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g576oa</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1g56pt5</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Fell into the Beetles gel trap</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g56pt5</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1g55v48</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Private label nail polish?</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g55v48/private_label_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1g55hiq</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Heartbroken: Lurid order disappeared</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g55hiq/heartbroken_lurid_order_disappeared/</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1g55di1</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Help finding dupe for Strength of Courage - Bee's Knees Lacquer</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g55di1</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1g55966</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fancy Gloss Hallows Eve Night </t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iqn4ick6n5vd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1g553kf</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Dollar store polish 💕</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqqdbkg0m5vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1g54uwk</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP Brightside is an excellent Halloween orange! </t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g54uwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1g54cu3</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Looking for minimalist nail art inspo!</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g54cu3/looking_for_minimalist_nail_art_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1g54b48</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Holo taco 🌮</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g54b48</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1g54anz</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Has the name of a polish ever swayed your purchase? </t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wb8bmxc3g5vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1g546i0</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Poison Apple Mani 🧪🍎</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g546i0</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1g53ukh</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>LynB got me again 😍🤩</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g53ukh</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1g53ka9</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Calling all Cauldrons, aka, Magic at Your Fingertips </t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g53ka9</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1g537oz</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>What is this orange substance in my nail polish?</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qpmcnxg385vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1g51xpg</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Nail art inspired by fake nails</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g51xpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1g51tzf</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Emily de Molly - disappointed </t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bo3v2gitx4vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1g511la</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t xml:space="preserve">OPI’s Nessie Plays Hide &amp; Sea-k </t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g511la</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1g51151</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>all I did was itch my leg!</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g51151</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1g50dhj</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Magnet discovery </t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g50dhj</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1g509a4</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>KBShimmer - Gummy A Break (reflective)</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g509a4</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1g4zklv</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Short nail bed</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rm3l2frvf4vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1g4z499</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Legit got like 100 compliments while wearing this!</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4z499</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1g4y232</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I was going for Frosty Fall Leaves </t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jf9pdf5i24vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1g4xq0j</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>ILNP Enchantment 😍</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3uxw9nxbz3vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1g4xk5z</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>wrap tipping question</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g4xk5z/wrap_tipping_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1g4xb7l</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>holo layers</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4xb7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1g4vzik</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Pretty manicure suggestions for olive skin tone</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4vzik</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1g4vy8e</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>What's up with the tree rings on my nails?</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4vy8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1g5ke5p</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blue abstract </t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5ke5p</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1g5k9mv</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Halloween nails 👻</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5k9mv</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1g5gxbt</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>First time using nail stands - game changer🩷 Spooky nails!</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5gxbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1g5fbuf</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Shmokey Nails🚭</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yrs9k3qyw7vd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1g5ex4p</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>I was trying to vibe for Italian Renaissance</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7m3nfgjat7vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1g5e202</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Been practicing my nail art </t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5e202</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1g5bs3v</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Nail School</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5bs3v</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1g5al91</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>I love this color! What do you think?</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1vnhgtor6vd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1g58gk0</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Freddy VS. Jason Tribute Nails 🔪🩸🚤🔥</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g58gk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1g57msr</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Happy (belated) National Mushroom day October 15th across the pond! 🍄</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/quu1y13256vd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1g57h2n</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>My nails in black. Beautiful!</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/915ovx4w36vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1g55zo1</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Ghastly, Haunter &amp; Gengar Nail Set for Halloween</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aflh78hms5vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1g52ar9</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Need advice to create Halloween werewolf feet</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wm7qva3c15vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1g50nvp</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lilac and glitter </t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hgnfnlepo4vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1g4wtc9</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky season, I didn’t have a small enough brush, last pic is inspo. </t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4wtc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1g4wq3e</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Saw these on Pinterest and tried for myself</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g4wq3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1g4iq2i</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Halloween</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/657n4cvalzud1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1g4piv2</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Nail ideas!</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7j35v0yq81vd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Oct 18 08:10:32 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_20.xlsx
+++ b/data/collected_data/2024_10_20.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C841"/>
+  <dimension ref="A1:C1030"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14730,6 +14730,3219 @@
         </is>
       </c>
     </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1g6czmk</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>I can't afford to do my nails anymore</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g6czmk/i_cant_afford_to_do_my_nails_anymore/</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1g6cyr7</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Just finished my autumn nails 🍂 took me 3 hours but it was worth it 🧡</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6cyr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1g6cuwr</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>My October nails</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o1qib7b51hvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1g6chy2</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glue gun glue for attaching 3D charms? </t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g6chy2/glue_gun_glue_for_attaching_3d_charms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1g6bild</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Practicing Painting</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6bild</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1g6bnp6</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nvxu697hkgvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1g6bm7c</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Just wanted to show my cute nails!</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxs940sxjgvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1g69jvx</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Acrylic nail lifting </t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g69jvx/acrylic_nail_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1g6a1su</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Please don’t kill me Mr.GhostFace, I want to be in the sequel😩👻</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6a1su</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1g68gpv</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Tips for finding salons with OPI?</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g68gpv/tips_for_finding_salons_with_opi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1g66sqp</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>dye resistant top coat?</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7um9ums3fvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1g681sh</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>My spooky set 👻</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n0g5s1jwffvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1g67zb2</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which polygel brand is better?? </t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g67zb2/which_polygel_brand_is_better/</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1g65f7e</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Need some inspo please!</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g65f7e</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1g67g3q</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Nails shape &amp; length</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rv77gh42afvd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1g67azu</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Is there any way to stop your nails from getting clear after a shower?</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wf4irpbp8fvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1g66s6f</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>My first time with press-ons. How did I do?</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ix9793en3fvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1g66fda</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>October nails</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g66fda</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1g663d5</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g663d5</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1g65qe5</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Nail techs - would you work on my nails?</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nnp3esdntevd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1g65mgq</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall/Halloween nails </t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tzobixfmsevd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1g65gqk</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>New set ❤</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1fef4u2revd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1g659tn</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Spooky Szn Spirit</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cjmsj5cbpevd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1g6508f</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>🎃🎃🎃</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6508f</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1g64op9</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t xml:space="preserve">@handjobsbyallison posted these on insta and I had to do them for myself - also lol at her handle </t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g64op9</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1g64vyp</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Classic and natural</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g64vyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1g6469y</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Acrylic nail come away from natural nail, what can I do I go on holiday in 2 days :)</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfkum2jmfevd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1g640ds</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>candy corns</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4tws3g8eevd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1g63szk</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>am i stupid? how long does it take your nail polish to dry?? 😭</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g63szk/am_i_stupid_how_long_does_it_take_your_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1g63dyl</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t xml:space="preserve">advice please </t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzn4jq4u8evd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1g63byq</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Freestyle Vacay Nails</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g63byq</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1g62wmb</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Inspired by The Phantom of the Opera 🌹</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g62wmb</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1g62rbi</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Pre-engagement nail help!! (Color inspo from insta names on each picture where found)</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g62rbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1g614op</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>What nail shape should I get</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g614op</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1g61v73</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Sheer “glazed” polish</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/61jah469wdvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1g61uf9</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>my journey 🤩</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g61uf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1g61r4y</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just did gel x for the first time </t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g61r4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1g61pg2</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Pink💓💓</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2bn56auzudvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1g61mu4</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Can you get a fill of a french tip acrylic set at a different salon?</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g61mu4/can_you_get_a_fill_of_a_french_tip_acrylic_set_at/</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1g61b7u</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Has anyone dealt with this?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9bze1ugxrdvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1g61ang</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t xml:space="preserve">$85 for this set </t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hecnovwrrdvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1g618j4</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Was under-spooked by my choice of purple at the salon. Luckily I found these nail stickers today to spook them up! Shout out to Flying Tiger</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g618j4</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1g60wpr</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ua250w5todvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1g60stv</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Ghostie nailsss</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ov5tbofzndvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1g60e02</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>broke the nail of my right pointer finger at the base but couldn't bear to cut them all that short; swipe for the original length that i kept on the other hand.</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g60e02</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1g6054y</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Nails for my client 🥰</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o38jdq8vidvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1g5z4s7</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>How do I convey what nails I want?</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g5z4s7/how_do_i_convey_what_nails_i_want/</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1g5zqut</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joining the Halloween spam. 🕸️What do you think of my 👀? </t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sylr9imufdvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1g5zg2t</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My birthday present from my amazing boyfriend! Medicool Pro Power 35k Portable Electric File with Erica Diamond Bits! </t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/02426d7jddvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1g5zd7g</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>White of nail going up the side?</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z9so4clwcdvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1g5zb2j</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Most basic autumn nails </t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5zb2j</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1g5yt4e</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Classic funny bunny 🤍🐰</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dndxxwrk8dvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1g5ypv9</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>MATTE BLACK W GLOSSY FRENCH GEL MANI 🖤</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32tq1qfv7dvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1g5ylqb</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Photo progression going under a tunnel. I am obsessed with this glow!</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5ylqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1g5yd2g</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>autumn gels 🍂🤎</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g05tvtz85dvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1g5yb8e</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>The Winter Soldier nails 🤩</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5yb8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1g5xz3x</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>My nails technician brought my Halloween dreams to life</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5xz3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1g5xwxn</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Halloween Nails! 🎃👻</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0yyzwyus1dvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1g5xqxs</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Koi fish nails by me</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wgck4iji0dvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1g5xogo</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love these Halloween nails! My guy nailed it! </t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5xogo</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1g5xn6z</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>What do we think about this shape? I was going for almond</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5xn6z</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1g5xjed</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>My Halloween nails 🧡🫶🏼</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0a193nwycvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1g5xamy</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Looks like we all got the bat nails memo this year</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5xamy</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1g5x0dh</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Simple nail design</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9emicvyvucvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1g5wpl7</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween elegance! </t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5wpl7</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1g5wcs7</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Nails for October</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4a4c88evpcvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1g5w6dr</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Looking for Nail Tech (Jackson, MI)</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6esfn5jocvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1g5vxdj</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What's the best nail design for a black outfit as a wedding guest. </t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g5vxdj/whats_the_best_nail_design_for_a_black_outfit_as/</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1g5vwe1</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Gel polish as glue?</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g5vwe1/gel_polish_as_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1g5vnhz</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>The difference of having a base coat?</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g5vnhz/the_difference_of_having_a_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1g5vmgk</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>new nails, what do u think?</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rrqvmfqfkcvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1g5vl75</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Cat eye🩸</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0leavir5kcvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1g5vfob</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do I do?? </t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g5vfob/what_do_i_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1g5vc2s</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this ombré as painfully bad as I think it is? </t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/macuhkn9icvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1g5vc0o</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Decided to go short and simple this time </t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aforyo79icvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1g5vbn6</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lol flower nails </t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5vbn6</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1g5vayd</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>My new nails</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aum4t621icvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1g5upok</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>My nails with glitter for the first time :)</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dmm5kylhdcvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1g5uhn7</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Help required</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5uhn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1g5tvy3</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Loving these marbles</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5tvy3</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1g5tkhb</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>2 hours with a master</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fx202nyi4cvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1g5t85u</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Gap between cuticle and nail?</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mddt4rs22cvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1g5t2h5</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can you paint over a full set at home? If so, what is the process? </t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45919hft0cvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1g5sb9k</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>First French Nails</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4uza6j0vbvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1g5s65d</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Seeking advice on products that can prevent nails from ripping as damage grows out. </t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5s65d</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1g5s2g6</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>First time polygel ombre (lazy girl method). As a rule of thumb, where should the pure pink stop in a babyboomer ?(The white spots I think are because of the alcohol and the white cured a bit clear.)</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qs5i27v2tbvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1g5rzgj</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>pls help</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3mbxid4fsbvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1g5sue2</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Really like how the tortoise nails came out this time</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5sue2</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1g5s8rk</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Joining the Halloween spam 🖤🕸️</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vuk5a6sgubvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1g5rxkn</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Having Nails Done</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g5rxkn/having_nails_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1g5rfus</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Got creative with my Halloween design</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5rfus</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1g5rc64</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Cracked nails</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lwt1srg5nbvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1g5r2i0</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New to nails, need ideas! </t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5r2i0</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1g5q9xw</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>First acrylic nails, what color should I use next?</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ck3oyvf2ebvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1g5q8j5</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>All time favouRED</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmqjtnyodbvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1g5pyt1</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Do you like my little ghosties? 🥹👻</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/30rpj5n4bbvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1g5pxbl</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>I got my nails done for the first time, what do you think?</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5pxbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1g5pusq</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Spooky season set #3</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kloklwu1abvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1g5p2r9</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FAV NAIL TECH </t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5p2r9</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1g5n7tb</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should I do the on the rest of my nails♥ ? </t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ee2ftdsmgavd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1g6akds</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cirque Catalina </t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6akds</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1g6agcv</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m kinda proud of this spooky set! </t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6agcv</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1g6adrp</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Atomic - Creepy Paper</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6adrp</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1g69zuj</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Recommendations for Black to Clear Thermal Toppers?</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g69zuj/recommendations_for_black_to_clear_thermal_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1g69wia</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black cat Halloweenish nails </t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g69wia</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1g69b2l</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>🍁 Finally Fall vibin🍂</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g69b2l</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1g691mq</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>dupe for lights lacquer emerald (creme formula)?</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cfw6iuztpfvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1g68qxo</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Arcana Lacquer - The Magician</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g68qxo</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1g67uhj</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Halloween nails</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g67uhj</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1g67iqz</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Tried a new combo out! 🍂✨</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g67iqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1g671h4</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Looking for a comprehensive, ranked list of indie polish recs!!</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g671h4/looking_for_a_comprehensive_ranked_list_of_indie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1g671by</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>orange for october ✨</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g671by</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1g66twj</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Pre-Halloween Mani &amp; Bonus Epic Fail</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g66twj</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1g666bo</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall multichrome </t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g666bo</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1g65k5t</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Mani I did for a wedding this weekend ❤️</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g65k5t</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1g65bs7</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Heart’s Desire</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g65bs7</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1g64m6z</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Colours like HoloT and MoonCat, but gel? </t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g64m6z/colours_like_holot_and_mooncat_but_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1g649vb</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Sabrina + the boys</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g649vb</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1g63q6x</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Rum Ham!</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g63q6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1g63hvv</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Replacement Brush Question</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9cqfsps9evd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1g63cjd</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sassy Sauce Chicago Fire + Kisses to my X’s!! </t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g63cjd</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1g62xki</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Essie special effects line - mulling over which to buy, would love Opinions</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g62xki/essie_special_effects_line_mulling_over_which_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1g624n9</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Can’t stop won’t stop</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9jl7f7ydydvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1g61y02</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Holo Taco “Berry Me in Holo” dupe</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g61y02/holo_taco_berry_me_in_holo_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1g617fz</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Did I achieve Velvet Nails?</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/utfax6q1rdvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1g616rc</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Is there a subreddit like this, but for makeup?</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g616rc/is_there_a_subreddit_like_this_but_for_makeup/</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1g60cxv</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I Have Finally Finished My Refill Bottle Of Seche Vite! </t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/071osrpikdvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1g604wh</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Watery 💧 </t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g604wh</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1g602qd</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>needed a palate cleanser after vampies and holos</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g602qd</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1g5znpd</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>I'm back with even more green and blue polishes added to my collection (I'm completely fine and normal)</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5znpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1g5z84e</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Prettiest shift!</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5z84e</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1g5z70s</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Dupe for Essence Space Glam</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5z70s</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1g5yyat</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Halloween nails👻</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5yyat</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1g5yt82</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>LynBDesigns Order/Delivery Question</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g5yt82/lynbdesigns_orderdelivery_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1g5yk4s</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you like candy corn? </t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5yk4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1g5yebs</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Fall is for Berry tones!</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5yebs</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1g5y96t</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thank you for your tips! Now mourn with me </t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5y96t</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1g5xxiw</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Loving this subtle, neutral flaky polish!</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5xxiw</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1g5xfgi</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Kelli Marissa Halloween Glitters</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5xfgi</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1g5xc1c</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>OPI Big Apple Red v. Essie Forever Yummy</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g5xc1c/opi_big_apple_red_v_essie_forever_yummy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1g5x3qg</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>twisted terracotta tanzanite</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5x3qg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1g5ww9g</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love how these butterfly/fall nails turned out </t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5ww9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1g5wn02</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Death Valley Nails - Varicose Veins </t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4mtv7z33scvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1g5wj8w</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>little bubbles in finished polish!</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5wj8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1g5w9g7</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>All my bridal era manis 💍</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5w9g7</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1g5w9cv</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>So sparkly I know it's marketed as limited edition and seasonal but it's an any timer for me</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7t3ka55pcvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1g5v8vl</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black Dahlia from Abomination Cosmetics </t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qao5liflhcvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1g5ttow</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Fall Manis</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5ttow</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1g5th5h</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Taco nails</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kaolzzez3cvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1g5tacr</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Bubble Bath 🫧</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izje3wdk2cvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1g5ta1h</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Press on help</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5ta1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1g5sws6</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Fall vibes</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ltfhda9ozbvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1g5sl3w</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Black cat eye polish, reminds me of the cosmos 🔭✨🌌</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ec80pq77xbvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1g5siut</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>My First Mooncat!</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5siut</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1g5sbcr</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Favorite 5-free polishes available at Walmart (Canada) especially base coats</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g5sbcr/favorite_5free_polishes_available_at_walmart/</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1g5s2ez</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Phoenix Indie- Bill</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oi4xssl2tbvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1g5ront</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Freshly Bitten 🧛‍♀️ 🩸 </t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5ront</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1g5rl61</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Nail polish similar to essie grow stronger base coat</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5rl61</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1g5r9ok</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Got creative with my Halloween Design</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5r9ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1g5r1ja</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>First time freehanding nailart! 🍁🍂</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/homf0xjokbvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1g5r15h</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I wish my camera could show you what I see! </t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0vzi5hekkbvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1g5qkej</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Spooky nails ¯⁠\⁠_⁠༼⁠ᴼ⁠ل͜⁠ᴼ⁠༽⁠_⁠/⁠¯</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5qkej</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1g5qhzl</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I Ain’t Got No Body and I need to talk about it. </t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vf6ecirzfbvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1g5qfp8</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monarch Lacquer Psycho </t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6cfcaioffbvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1g5q5e6</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>All time favouRED</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdcar5wvcbvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1g5okcp</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Quick nude manicure</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5okcp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1g5o3v9</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Fall mani</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tymdeq3lravd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1g5ml4u</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>🍂 Fall mani</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rmpmjrx58avd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1g5mkjm</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>OPI Holiday 2024 x WICKED: "Ozitively Elphaba"</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5mkjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1g5dzln</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Looking for a Warm-toned Red Cream</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g5dzln/looking_for_a_warmtoned_red_cream/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1g5fusk</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Werid question, does it feel like your nails can't breathe when you where polish?</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g5fusk/werid_question_does_it_feel_like_your_nails_cant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1g69h7q</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Easier ways to do this?</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7fyotdvgufvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1g6902v</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Stitch nails</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6902v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1g68pge</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>This might be a new favorite! Took me a while but I think it was worth it! Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2z795s4amfvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1g681c7</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Loving my new nails ❤️</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0bby4gurffvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1g67dm8</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Rate my Halloween nails?</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g67dm8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1g66nt6</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Second Halloween set</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g66nt6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1g65k6j</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>My Halloween Nails what do you guys think?</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tx8tr1e0sevd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1g61r41</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Pink💓💓💓</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3sl48xvcvdvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1g5z2w0</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Halloween nails 👻</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5z2w0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1g5y58e</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Guys, be honest please, is this too much? </t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dje65cul3dvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1g5xq32</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>They were so perfect</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fvrqpo630dvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1g5x5su</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Wing away</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5x5su</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1g5x05h</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just wanted to show my 1 year progress </t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5x05h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1g5wud1</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Halloween fun</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5wud1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1g5tury</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Loving these marbles</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5tury</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1g5s5hu</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>My Freddy K 🔪 Pressons</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5s5hu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1g5nl18</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails! </t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g5nl18</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1g5mppo</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>How do we feel about these?</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/17nzxums9avd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Oct 19 08:09:32 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_20.xlsx
+++ b/data/collected_data/2024_10_20.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1030"/>
+  <dimension ref="A1:C1204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17943,6 +17943,2964 @@
         </is>
       </c>
     </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1g744n6</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Green speck on my ring finger nail</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bs7mxe497ovd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1g73wcf</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Wedding Nails</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g73wcf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1g73jfe</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall af </t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g73jfe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1g6suzu</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time square/squovel instead of oval/round </t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6suzu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1g6svlc</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Apres Gel X kit VS Light Elegance tips with Jimmy Gel??</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g6svlc/apres_gel_x_kit_vs_light_elegance_tips_with_jimmy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1g6w5mw</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Need some inspo for November Nails!</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sd0npm1brlvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1g73d34</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying different colors for french tips♥ </t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bljkrf9nwnvd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1g739zo</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>I love Halloween, and being in a cast isn’t stopping me! I love my nail tech 🥰</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g739zo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1g737qe</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Fun Halloween nails</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xp1iopisunvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1g735mj</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Cat Eye 😆</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sv4bb3t0unvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1g730zr</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>My first Halloween set🕷️🧡</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g730zr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1g72t62</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>First time in years I've had a short gel mani</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6kupl9lepnvd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1g72p7r</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>I busted out the magnet for my Halloween nails 🎃</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l68z7loynnvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1g72hy1</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>I love the results</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8lwgn82clnvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1g72as4</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Spooky nails and even spookier poses 👻</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g72as4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1g72482</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>E file recommendations</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g72482/e_file_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1g71xr3</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Another witchy fall set of nails. My tech has some serious talent with the paint brush! (Naturally Nails in Clayton, BC) </t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/015n20a6envd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1g71ghy</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Acrylics vs Dip Nails (Which Do You Prefer)? </t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g71ghy/acrylics_vs_dip_nails_which_do_you_prefer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1g712i3</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Game Day Nails! Old set but I just joined the sub </t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g712i3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1g70qk8</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>My October nails</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6wwsxtve0nvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1g70bzc</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g70bzc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1g6trio</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bungo stray dogs free style </t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwg5susk6lvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1g6ww85</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Nightmare Before Christmas inspired nails</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6ww85</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1g6vj9p</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Nailpop: is the Temu/AliExpress brand any good?</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6vj9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1g6s5pj</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for advice, please help! </t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/axi4p975tkvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1g6sset</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>❤️Red Nails❤️</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6sset</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1g6zquh</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>🖤💚</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zz12kbwpmvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1g6z2gn</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Season of the Witch 💫 </t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtrtxap1jmvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1g6z1sz</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Delicate💅🏼</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6z1sz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1g6z0l4</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>october nails 💚</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7gx9h24iimvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1g6yn8e</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>I ❤️ ME</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6yn8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1g6yn3m</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Strong nails</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g6yn3m/strong_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1g6ykk4</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Going to Tokyo next week, nail salon suggestions?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g6ykk4/going_to_tokyo_next_week_nail_salon_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1g6ye6z</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>I guess it’ll work…</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6ye6z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1g6ye6t</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Second Halloween set 🎃</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dclawuz9cmvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1g6xxpr</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My October nails!! </t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6xxpr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1g6xts1</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Halloween nails 🦇</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6xts1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1g6xrmt</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>First Attempt w/ Polygel</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6xrmt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1g6xl9n</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>What’s black, white &amp; red all over ‼️</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f4ummlri4mvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1g6vpe8</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Fall Green Colors</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6vpe8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1g6vlrh</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>My nail tech killed it. Loooove these 🖤</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5uoqryqdmlvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1g6vjmf</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Trying something different</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fa4q2fpullvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1g6vdru</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>I can never decide between gloss or matte polish but I’m so happy with how these came out 🎃</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6vdru</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1g6v5lq</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My 13 year old daughter did these herself. I told her y’all might appreciate them. </t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p7v0mpneilvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1g6v0ec</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>trying out some more charms! what do you think?</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/91r4mdx2hlvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1g6uynz</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Finally had time to do my nails this semester</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3dj8buoqglvd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1g6uute</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Disappointed first hard gel mani</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6uute</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1g6uq1n</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/km7lkq4oelvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1g6tzid</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherry nails! </t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6tzid</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1g6tw05</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Hate feeling of files and buffer</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g6tw05/hate_feeling_of_files_and_buffer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1g6tdlv</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Hard Gel/Gelx question</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lzub1ehe3lvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1g6t7xg</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thank you u/dankmachinebroke for inspiring my nail tech lol I love this design </t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kc6j2vu42lvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1g6t6s6</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Halloween part 2 of nails😍💅🏼🎃🕸️🦇⚰️</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zunzi0wv1lvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1g6sxe2</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>1 o 2 ? 🖤 Gothic style❤️</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6sxe2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1g6swvx</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Is this color too dark on me?</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6swvx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1g6sw7i</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Gel removal?</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/detmr51gzkvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1g6sqao</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween Nails! </t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6sqao</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1g6skn3</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>I've started doing my own nails - thoughts?</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6skn3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1g6shr6</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Eras Tour Nails!</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6shr6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1g6shit</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Why do some subreddits gatekeep natural nails? Incoming rant…</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g6shit/why_do_some_subreddits_gatekeep_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1g6sdid</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>how much should i be spending on a bottle of gel polish?</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g6sdid/how_much_should_i_be_spending_on_a_bottle_of_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1g6sas3</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY: second attempt at mag with “moonlight” mags </t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vomc5f04ukvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1g6rb01</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Essie Kiss and Spell, Essie Gel Setter taco (highly recommended both)</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://imgur.com/mXhdYmd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1g6qzd6</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t xml:space="preserve">halloween and vampire vibes </t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b3cv1npwjkvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1g6qz3q</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Had to get them redone</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okjkodyvjkvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1g6qm6x</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stained glass nails advice </t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uphpbr52hkvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1g6qe2l</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Fresh set and I’m so happy with them</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ozljbrbbfkvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1g6qe0r</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t xml:space="preserve">*NOT MY DESIGN* need to find this shade of pink </t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3tccjnxafkvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1g6qdl7</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Pink Unicorn Chrome</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6qdl7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1g6qdaf</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Got gel nails for the first time</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ru4q47h5fkvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1g6qagd</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Friday the 13th nails</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6qagd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1g6q946</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Cloudy Night ✨☁️</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6q946</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1g6psgz</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6psgz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1g6p2c2</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Final results first time doing gel x + french</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6p2c2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1g6oru5</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Back to purple cuz my hope is back!(hobi💜).</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6oru5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1g6olyb</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Any tips to shape coffin nails?</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0623d5nn1kvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1g6oimo</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>😋🤎</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/52c8p7fy0kvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1g6nwao</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this normal? </t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6nwao</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1g6npj2</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>First time</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6npj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1g6nn0e</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Thought I’d switch it up.. what do we think!? 👍 of 👎</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6nn0e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1g6njz9</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Accidentally injured my nail using drill</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eahqynhntjvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1g6niby</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>What am I supposed to do with this?</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ahznltoatjvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1g6m4h8</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do we think? 🤔 </t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6m4h8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1g6mzku</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">October thangs </t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hg5g41lcpjvd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1g6mrsv</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Does biab make anyone else’s nails really weak?</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g6mrsv/does_biab_make_anyone_elses_nails_really_weak/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1g6mmyr</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>First kitty and new kitty nails</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6mmyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1g6mlgt</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Fresh set</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/erjkmj6dmjvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1g6miqp</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Cute Spooky eyesss</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m075wpwrljvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1g6lzxa</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Obsessed!</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6lzxa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1g6llks</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Don’t hug me I’m scared nails!</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b86uvcxzejvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1g6lh3t</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Autumn Espresso 🤎🤍</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6lh3t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1g6l6hh</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">honest opinion </t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mghz6r5cjvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1g6kx02</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Had a tough week so took today off to treat myself. I haven’t had acrylics in a long time and these came out so cute!</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qkjgt60majvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1g6kamb</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>First time freehanding nailart! 🍁🍂</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ee5m6kw5jvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1g6fqep</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>How do I keep anything on my nails???</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g6fqep/how_do_i_keep_anything_on_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1g6isyr</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Why is my top coat going matte?</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08xggxp9uivd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1g6kef3</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My october nails </t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/712w1ugp6jvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1g6kbn1</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">waiting for halloween </t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3q6ygjq46jvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1g6k769</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pup is unamused but here’s my fall fave: LPAD </t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6k769</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1g6k2c4</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Builder Gel or Gel x?</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6k2c4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1g73yv0</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>How to protect nails whilst cleaning the house? (Besides a fresh mani and gloves)</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g73yv0/how_to_protect_nails_whilst_cleaning_the_house/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1g7379c</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Are there any alternatives to builder gel for nail strength I can use if I'm allergic?</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g7379c/are_there_any_alternatives_to_builder_gel_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1g72nft</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A sparkly Halloween manicure </t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g72nft</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1g72kwy</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>my (finger/toe)nails are literally peeling from the cuticle</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g72kwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1g71oto</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Rudeness of the comments aside —- Why did no one mention the blood splatter all over the carpet???</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g470hp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1g71o1y</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Night Owl Lacquer - Heart of a Dying Star</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g71o1y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1g70nim</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>ghostly and seasonal</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g70nim</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1g6zb7y</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Cozy Cuff Season for the Foreseeable Future</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8kk8q5ohlmvd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1g6y9i5</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>new eyeshadow palette had nail polish as a bonus</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z21rjn90bmvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1g6y930</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Does anyone know of a pink/magenta shimmer topper please 😭❤️ Doesn't have to be this exact shade of pink/magenta</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/it7tok5wamvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1g6y808</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kbshimmer is raising some of their prices </t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2uvkbtlamvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1g6y0af</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Loving this Paradox from cirque colors.</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6y0af</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1g6xrmd</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>In your experience, is Cutex ultra-powerful/gel nail polish remover better than 100% acetone?</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g6xrmd/in_your_experience_is_cutex_ultrapowerfulgel_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1g6xknx</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>JEWEL BEETLE IS SO PRETTY</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6xknx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1g6xe7s</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Orange jelly sammich on shorties for spooky season</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6xe7s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1g6x5wr</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>INLP- Pyro</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r44iqhjj0mvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1g6wy1t</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fave indie FALL colors for SHORT nails! </t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g6wy1t/fave_indie_fall_colors_for_short_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1g6vygf</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>swatch comparison request</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g6vygf/swatch_comparison_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1g6vvyw</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t xml:space="preserve">do glow in the dark polishes die like thermals? </t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7d4hzpixolvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1g6vv2k</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Opal Nails</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dw9c8ablolvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1g6vi7p</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>PlumbLuck Dupe</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7fa7fmhllvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1g6vagt</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>I'm new to this...</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uclcz5fkjlvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1g6uwiv</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>A poisoned apple a day keeps the happily ever after away 🍎☠️🥀</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6uwiv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1g6sm2g</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Velvet nails? For Fall? Groundbreaking. </t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/000juo8nwkvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1g6s8oo</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Orly Colorpass Winter 2024</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6s8oo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1g6rhz9</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>👹 HAIL KITTEN 👹</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6rhz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1g6r7jv</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Some of my saddest breaks</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6r7jv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1g6r1ul</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Questions about Long nail beds</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g6r1ul/questions_about_long_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1g6pyyb</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail color </t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g6pyyb/nail_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1g6ppze</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Mooncat Queen of the Dead</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0ni3c3l6akvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1g6pn7j</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Thank you!</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6pn7j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1g6pbc0</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The shining </t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6pbc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1g6p9xd</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Let 'em Roar 🦖</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0t9a7drr6kvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1g6okpt</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Bad start to October</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxm6nrsd1kvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1g6ockh</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Fall is for skittle manis</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgwfjhjqzjvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1g6oc9w</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>I love using sheer polishes as a topper</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5k5qjk0ozjvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1g6o68a</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Got my Fancy Gloss order...</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6o68a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1g6o0zi</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Burgundy with Blue/Teal Shimmer</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g6o0zi/burgundy_with_blueteal_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1g6nucj</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Thrifted 4 Chanel polishes for $1 each! They seem new to barely used.</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fyc73thqvjvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1g6n997</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>A Tale of red-brown-base-with-glowy-green-to-blue-shimmer</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6n997</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1g6mldo</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">We’re supposed to hold the bottle, right? </t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6mldo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1g6ml0d</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Speedy thing goes in, speedy thing comes out.</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxm48rl9mjvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1g6lufn</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Cured by Julep Take a Breather Oxygen Nail Treatment</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ut23mvpgjvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1g6l6oe</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t xml:space="preserve">30lb horseshoe magnet price? 🧲 </t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g6l6oe/30lb_horseshoe_magnet_price/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1g6kz8v</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>rosalie</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6kz8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1g6kspg</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>First Halloween mani of the season 👽🧙‍♀️🎃</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/80cenlsq9jvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1g6kocq</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first magnetic polish! </t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3jbbe7xi8jvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1g6jwv1</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Video doesn't do this color shift justice!</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/itlsmzzx2jvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1g6jil4</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So I apparently have a problem. I like to use swatch sticks to test out different combos and whatnot, and then I don’t write anything on the stick. I have like 100 of these and no idea which polishes I used lol. </t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywvy7hmxzivd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1g69g68</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Emily de Molly - Leave a Light On VS Phoenix Indie - You Always Be My Sister</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g69g68</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1g6avfy</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Jojoba Oil vs Hard as Hoof?</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g6avfy/jojoba_oil_vs_hard_as_hoof/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1g6gtep</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Any dupes for this polish? Color “Desire”</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g99apgz3divd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1g6im7p</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>ABCs of polish! W is for What Addiction.</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2w8i8nhssivd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1g6hfe9</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>SIN EATER 😈</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6k3v68oqiivd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1g6g085</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails will not soak off - MMA? </t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g6g085/nails_will_not_soak_off_mma/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1g6dc7c</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>ILNP Rosewood + the Alchemist</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgy07jux7hvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1g71abx</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Someone said my nails were ugly😫😫😫</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r467mkuj6nvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1g70vwy</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jujutsu Kaisen Nail Press on Order! </t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g70vwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1g6zi9w</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Looking for Feedback on My Press-On Nail Designs</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1g6zi9w/looking_for_feedback_on_my_presson_nail_designs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1g6yi51</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Tried dried fall leaves 🫠</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6yi51</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1g6y5xx</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t xml:space="preserve">halloween club </t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6y5xx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1g6xyo3</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying to hand paint! </t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6xyo3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1g6wogq</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Spooky voodoo nails for Halloween 🎃</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6wogq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1g6wbfi</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>beginner falloween nails</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6wbfi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1g6w9b3</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New spooky set! </t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6w9b3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1g6vw2t</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wizard of Oz Nails </t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4z9c8lhxolvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1g6tznh</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🧡 </t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xhhssngf8lvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1g6ta2b</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Just a desperate parent trying to make their daughter happy. Help me?</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1g6ta2b/just_a_desperate_parent_trying_to_make_their/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1g6s1sx</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Chucky!</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tm2c3b1askvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1g6qqws</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Pink Unicorn Chrome</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6qqws</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1g6mbxt</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do we think? 🤔 (nails done myself) </t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g6mbxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1g6lwrk</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>I got these today, basic but cute. 🖤</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t8xu3qe7hjvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1g6cxqf</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Nails for my girlfriend</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1g6cxqf/nails_for_my_girlfriend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1g6hskq</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Halloween Set</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ya8lululivd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Oct 20 08:10:21 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_10_20.xlsx
+++ b/data/collected_data/2024_10_20.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1204"/>
+  <dimension ref="A1:C1401"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20901,6 +20901,3355 @@
         </is>
       </c>
     </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1g7tkr0</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>my new nails</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7tkr0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1g7th42</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Frankenstein Vibes</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/da688tvk7vvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1g7ssuv</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did this yesterday </t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/opu1ztfjyuvd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1g7sg33</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Warm autumn nails</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6dc7sc2xtuvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1g7s5ai</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>pick your favourite nails. 💘🤝</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7s5ai</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1g7s23z</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t xml:space="preserve">obsessed </t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mu22gpitouvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1g7rn6r</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pick a color pls I'm indecisive. </t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8725cg4kjuvd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1g7qyzv</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>My simple little treat - manicures</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzhp2jtabuvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1g7qsht</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Good night </t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xhimy0669uvd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1g7q9qn</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Halloween nails</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7q9qn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1g7pln0</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>First try with gel nails</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/umcej5k0wtvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1g7phko</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Wistful Water Lily 💅</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nm0bw2prutvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1g7oxk6</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Halloween nails</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/09q7pcnqotvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1g7oee9</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Where can I find Tomicca ULTRA short nail tips?</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7oee9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1g7oci5</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Tortoise shell nails</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7oci5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1g7o6oe</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>🪦✨😌</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c0tt1364htvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1g7o22d</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m very excited to see Korn on Monday if you can’t tell. </t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7o22d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1g7nvfy</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Fall Nails 🍂</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7nvfy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1g7nph6</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Behind on spooky season </t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7nph6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1g7nj2n</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>First gel x I did on my friend’s</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7nj2n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1g7nj0k</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Is this gel manicure too far from my cuticle?</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7nj0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1g7nh5d</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Unreasonable?</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g7nh5d/unreasonable/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1g7n238</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Almond Nails Breaking</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/it4tqo8w5tvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1g7n0ic</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky season! </t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7n0ic</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1g7m7tj</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ombré chrome nails &lt;3 I absolutely adore my nail tech 💅 </t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7m7tj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1g7m011</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Treehouse of Horror XXVIII 😆</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7m011</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1g7lzgx</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>how do we feel about textured nail polishes?</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxjm9ksmvsvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1g7lz9o</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Switched from acrylics to gel x extensions!</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e4cn8xrkvsvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1g7lxxr</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Decided to try and use builder gel to make a snake and koi fish!!</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/875jgiy7vsvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1g7lw3a</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>3d Hand sculpted Pumpkin 🎃 Should I make it matte? 💕</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2sz322vpusvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1g7led9</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural Nail advice </t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g7led9/natural_nail_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1g7l1d2</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Used pigment powder and a brush to create faux-airbrush sweater-y stripes!!</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7l1d2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1g7kdho</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Can I use builder gel with the polygel method?</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g7kdho/can_i_use_builder_gel_with_the_polygel_method/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1g7klcd</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Why are my nails turning white?</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06cdkxlbjsvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1g7koew</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Green chrome 🧪🧙‍♀️</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7koew</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1g7klw8</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>My preschool students chose my nail colors 🥰</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xlbl5hggjsvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1g7kk1c</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Halloween nails🤍</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7kk1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1g7ki51</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First attempt at nail art - beach. Any tips for next attempt? </t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wpybbb1iisvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1g7keb0</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>I’m a little colourblind, which of these is better for a halloween orange?</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8htvkj6ihsvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1g7k9is</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>halloween set!!</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7k9is</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1g7k347</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>My first post with Halloween nails!</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7k347</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1g7k1n4</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>WIP - My Halloween Set</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3oz034wcesvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1g7ikxr</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Why is it such a big deal that I prefer regular polish over gel?</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g7ikxr/why_is_it_such_a_big_deal_that_i_prefer_regular/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1g7gyg3</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can lamps lose strength over time? How can I know if my gel is absolutely 100% cured? </t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g7gyg3/can_lamps_lose_strength_over_time_how_can_i_know/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1g7gsca</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome powders not sticking to top coat </t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g7gsca/chrome_powders_not_sticking_to_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1g7j1zw</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>New Halloween set!!! 😍😍</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/asfjj0ys5svd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1g7j0un</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Vampire Nails 🧛🏼❤️</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7j0un</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1g7iyca</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not lasting </t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g7iyca/not_lasting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1g7ivqm</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Night and Day</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7ivqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1g7ijrn</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>First time using Gel X and doing nail art, thought I’d match my new pups nails :)</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7ijrn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1g7iihs</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Fall nail time!</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yv01duy31svd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1g7ihlr</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Minimalist Fall Nails</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7ihlr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1g7idya</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>It’s CORN 🌽</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d3qp2ii10svd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1g7hyo9</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Wedding nails! What do you think? Oh</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7hyo9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1g7hxq6</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Spooky Season Nails! 👻🎃</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7hxq6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1g7hvss</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>First Time Doing Gel-X Nails</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lbo07c0rvrvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1g7hvnu</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>SHEIN Nails</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g7hvnu/shein_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1g7hpen</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Hi!💖1️⃣,2️⃣,3️⃣ o 4️⃣❓💖</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f0d8rne7urvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1g7hpbz</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Unicorn acrylic nails</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iinlywm7urvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1g7hfvh</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first homemade long nails </t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08pio5vzrrvd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1g7h60a</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>I loved my new design 🥰😍.</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7h60a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1g7h5c0</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Summer is around the corner… and I had to have this colour….. thoughts</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5kgktsloprvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1g7gzll</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>A memorial set for my friend’s late brother.. 🤍 (with permission to post)</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7gzll</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1g7gz4v</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>What could have changed my nail color this way?</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7gz4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1g7gw3m</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Spooky Season Nails</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7gw3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1g7gtrd</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>These are the nails I got the other day</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7gtrd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1g7gqg6</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Gilded Cappuccino ☕️✨️</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7gqg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1g7fgxm</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Saw some inspo on Printerest and knew I had to get them.</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7fgxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1g7g7jn</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Chocolate &amp; tortoiseshell accent nails for fall 🍁🤎🍂</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7g7jn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1g7gcjm</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7gcjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1g7g42t</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Halloween Nails 👻🕸️</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7g42t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1g7fx0g</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Simple Halloween Nails💅🏻✨</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z3w4kdnifrvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1g7fw4w</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Dragons and flames</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7fw4w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1g7fr83</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>I just started and I’m definitely no professional but I’m proud of my work</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wkh1mzj6ervd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1g7fnik</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>coraline nailz🐈‍⬛⭐️🌀🕸️</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7fnik</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1g7f4cs</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>He approves!</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7f4cs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1g7ex4z</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Simple Halloween Themed</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvyr84tc7rvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1g7ett2</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Static Nails remake</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x22abb6k6rvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1g7epog</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I decided, what do you think for Halloween? I still have time to make another model </t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s31v91fn5rvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1g7eoi2</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>I don’t know what to do…</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7eoi2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1g7enph</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spooky Season is here </t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/prxd77k75rvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1g7dq8u</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time in 10 years! (Plus how my nails looked before 🫥)</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7dq8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1g7dq7x</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>My new nails!</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7dq7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1g7d78j</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Now can I say I'm cool? Haha feeling young again haha </t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23tomwehtqvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1g7d3ks</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t xml:space="preserve">natural nails </t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y1dmtq4msqvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1g7cny8</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Recommend Dip Powder (Netherlands)</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g7cny8/recommend_dip_powder_netherlands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1g7chxc</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Did these last year today💜</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7chxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1g7cewm</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Slightly wonky Halloween nails</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i76h7ikzmqvd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1g7bhpq</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dashing Diva nail wraps </t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1g7bhpq/dashing_diva_nail_wraps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1g7caxo</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>october nails 😁😁</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7caxo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1g79ena</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t xml:space="preserve">July 21st-October 19th growth progress, all Kokoist </t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g79ena</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1g7amrg</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0qrdwpe8qvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1g7b1tv</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Halloween Nails 👻🎃🕷️</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7b1tv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1g77ahn</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>How do I make sets last longer?</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g77ahn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1g7c01d</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>My Halloween Set</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7c01d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1g7bcxo</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Nightmare on Elm Street nails for Halloween using full coverage gel tips</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7bcxo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1g7acr8</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>My first Halloween nails of the season 😁</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7acr8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1g7ac71</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wanted to do Halloween nails but that’s just not my aesthetic- this is what I ended up with </t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7ac71</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1g7a9sa</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Mandarin time 🍊</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7a9sa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1g7a7fs</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c0bj6j4p4qvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1g7t7ty</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t xml:space="preserve">can I achieve this with regular nail polish? </t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/en6zvj5z3vvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1g7sy65</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Labradorite - By Dany Vianna, By Vanessa Molina, Whatcha collab</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7sy65</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1g7sxs7</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Okay, I'm sold</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7sxs7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1g7r2y9</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>💖💚Wicked Nails💚💖</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7r2y9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1g7qznx</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>How did I Fall in love with you</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7qznx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1g7q5c1</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>you guys…the new cirque collection is insane 🤩</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c7v4pg7z1uvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1g7pnym</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cadillacquer's Everlasting Storm </t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7pnym</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1g7paq4</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🍂 🍁 </t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7paq4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1g7ovi3</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>I have ADHD and I reentered a short, low maintenance phase. Loving this cute set.</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7ovi3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1g7om32</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Sparkling Indecision</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/npugldngltvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1g7oe05</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Does anyone know of a pearlescent polish like OPI I Meta My Soulmate but just slightly cooler pink or pink-purple? (Photo Swatch Credit: Gingerly Polished)</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddg676m8jtvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1g7nw8g</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Fall Nails 🍂</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7nw8g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1g7nsqc</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Show me your favorite nude I’ll show you mine? </t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7nsqc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1g7n404</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Advice please- transition from SNS/powder to other options.</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g7n404/advice_please_transition_from_snspowder_to_other/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1g7muov</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it orange, is it pink? Depends on the lighting. </t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7muov</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1g7lzvr</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blood splatter nails on my client </t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7lzvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1g7lzr0</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>First time trying magnetic polish!</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j14hgxcpvsvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1g7lv8z</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>blessed with beauty &amp; rage ✨</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7lv8z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1g7lt0a</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Leave A Light On </t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7lt0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1g7ldqy</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Queen of the Dead 🧛‍♀️</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l5pm5fkdqsvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1g7koi6</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Fairy vibes</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7koi6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1g7knsr</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>ILNP “Poison” is one of the magnetic GOATs</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1t2mecuxjsvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1g7kbhp</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Gilded Neutral ✨️🏛</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7kbhp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1g7k6ky</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Trying out different hand poses for pictures</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7k6ky</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1g7k4xs</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>DVN Swamp Sparrow</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7k4xs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1g7k0d9</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Need Opi pink polish gel with blue undertone</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g7k0d9/need_opi_pink_polish_gel_with_blue_undertone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1g7dy0y</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Peek-A-Blue - Salon Perfect</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7dy0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1g7j7fo</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Bloooddd. Stop saying blood to strangers.</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7j7fo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1g7iwqx</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Nail polish with colors similar to bright and colorful song birds?</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7iwqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1g7irzr</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What does kerasal actually help with/do? Does it help with inflammation? </t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g7irzr/what_does_kerasal_actually_help_withdo_does_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1g7irbi</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pure satisfaction w/Zoya Amy </t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljndmkh63svd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1g7iogm</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cirque colors support question </t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g7iogm/cirque_colors_support_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1g7igdx</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday nails </t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7igdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1g7ifjg</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>My sister got these done and I'm in love</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7ifjg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1g7hl2h</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Counting down the days to summer 😎</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7hl2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1g7hd94</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>KB Shimmer - It’s Fall Good 🍎🍂</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7hd94</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1g7h80n</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Haunted Forest by Mooncat</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nursy278qrvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1g7h5pd</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>🍂 Sparkly Fall goodness</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qpj3sjprprvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1g7h1rv</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I did it again! </t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iq24js6torvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1g7gtc9</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Matte glitter skittle</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7gtc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1g7g9so</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>I really wanted to love my first non-mainstream (KBShimmer and ILNP) polishes...</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g7g9so/i_really_wanted_to_love_my_first_nonmainstream/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1g7g0x8</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>First nail art design!</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w4tv1awcgrvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1g7fmp6</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ghostly nails for halloween </t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7fmp6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1g7fh7j</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Same polish in both pics. Literal magic.</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7fh7j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1g7ffi4</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>I still love color changing gel</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yq2mmifibrvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1g7f1hv</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Making spooky colors using existing collection 🦇</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x8tlc7b48rvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1g7f1de</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Let’s Hang</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bl1efiia8rvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1g7eygn</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail artist killed these </t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7eygn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1g7ewtl</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>A truly pale pastel mint blue</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7ewtl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1g7ecx6</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>Peely base question</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g7ecx6/peely_base_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1g7e3rf</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>What are your best tips &amp; tricks for nail prepping?</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g7e3rf/what_are_your_best_tips_tricks_for_nail_prepping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1g7defe</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>LynB Fair Isle Dupes/Cousins?</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7defe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1g7ddak</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Reddit Banner Contest Voting</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g7ddak/reddit_banner_contest_voting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1g7d828</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>How are you doing your nails for Halloween? 🎃 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g7d828/how_are_you_doing_your_nails_for_halloween/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1g7d6a8</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Was not expecting to be this into orange</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hv8doc69tqvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1g7ci3j</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Magnetic for fall</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7ci3j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1g7bzs6</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>How many of you don’t use a base coat? Concerned about damaged nails if I don’t use one</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g7bzs6/how_many_of_you_dont_use_a_base_coat_concerned/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1g7by2n</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>My first time trying aura nails</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11cckqd7jqvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1g7bvhf</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Fall nails! First manicure post.</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7bvhf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1g7buoa</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Do you magnetise all coats or just the last coat?</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g7buoa/do_you_magnetise_all_coats_or_just_the_last_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1g7btl5</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>You people are the worst</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g7btl5/you_people_are_the_worst/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1g7bi2e</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Dashing Diva nail wraps</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g7bi2e/dashing_diva_nail_wraps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1g7bfe6</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Spooky season shimmer</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xwnb7onxeqvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1g7bds4</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>[Looking for a dupe] Can someone help me find a regular nail polish on the shade "DND Flower girl"?</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g7bds4/looking_for_a_dupe_can_someone_help_me_find_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1g7bcwy</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>By far the best manicure I have given myself</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7bcwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1g71qky</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should I get gel or acrylics? </t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g71qky/should_i_get_gel_or_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1g79rco</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Purple or green? </t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x0dco8bn0qvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1g78z1d</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thanks for the LA colors drop tip-off, get you to dollar tree if you haven’t! </t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g78z1d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1g78leq</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Simple halloween themed skeleton french tips</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g78leq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1g78e4e</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Madeline 🖤</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r43lqni0opvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1g761zy</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Do you know space themed / night sky / galaxy nail polishes?</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1g761zy/do_you_know_space_themed_night_sky_galaxy_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1g7rqjb</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>Help! I need a new LED nail lamp. What do you recommend?</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i62avk8pkuvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1g7q1aw</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Halloween set!</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7q1aw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1g7pn5g</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Spooky Szn Nails</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7pn5g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1g7p382</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>lil diy ghosts</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7p382</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1g7onde</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Night and Day</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7onde</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1g7ogk8</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Tortoise shell nails</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7ogk8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1g7nwny</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Fall Nails 🍂</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7nwny</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1g7n52b</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>How to get crusty nail glue off?</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/teek02bo6tvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1g7lvca</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>3d Hand sculpted Pumpkin 🎃 Should I make it matte? 💕</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pz9hwoyiusvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1g7klso</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>Dragonglass</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wpa18icfjsvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1g7kgg5</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>What do you think? 🐄</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7d4k902isvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1g7k44t</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>I Still Love Color Changing Gel</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0k3f6ajzesvd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1g7k2wx</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>I went for the option D</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yaddnskoesvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1g7jxe6</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Halloween Hello Kitty 🎀</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7jxe6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1g7jvui</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Scream Press Ons </t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7jvui</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1g7jczy</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>Spooky season! 👻🕸️🕷️</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7jczy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1g7h4is</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t xml:space="preserve">They are so cute </t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9sb4nqqfprvd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1g7gtaw</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So proud to say I made them -they are so beautiful </t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvm05gysmrvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1g7gsmd</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome powders not sticking </t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1g7gsmd/chrome_powders_not_sticking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1g7gid8</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A or B or C? </t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7gid8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1g7fuf7</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Dragons and flames</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7fuf7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1g7eufu</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These took 5h 30 min. How can I be faster? </t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7eufu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1g7dfbc</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>🎃👻</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5jlk02bvqvd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1g7aq8k</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>second set ✨</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g7aq8k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1g766ik</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>first time trying spooky designs :)) (more coming) they're a little wonky but they're cute</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1g766ik</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1g75gab</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>I did my own nails!</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2poochmtpovd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>